<commit_message>
split A B C D Channels
</commit_message>
<xml_diff>
--- a/doc/PIN_REVERSE_ENGINEERING.xlsx
+++ b/doc/PIN_REVERSE_ENGINEERING.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="214">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="215">
   <si>
     <t xml:space="preserve">FMC Signal Name</t>
   </si>
@@ -664,6 +664,9 @@
   </si>
   <si>
     <t xml:space="preserve">Sampling time ns</t>
+  </si>
+  <si>
+    <t xml:space="preserve">num of periods sampled</t>
   </si>
 </sst>
 </file>
@@ -2270,16 +2273,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F9" activeCellId="0" sqref="F9"/>
+      <selection pane="topLeft" activeCell="D17" activeCellId="0" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="18.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="21.64"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2295,8 +2299,11 @@
       <c r="D1" s="0" t="s">
         <v>213</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E1" s="0" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
         <v>125</v>
       </c>
@@ -2310,6 +2317,19 @@
       <c r="D2" s="0" t="n">
         <f aca="false">B2*C2</f>
         <v>8192</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <f aca="false">1000/A3</f>
+        <v>66.6666666666667</v>
+      </c>
+      <c r="E3" s="0" t="n">
+        <f aca="false">D2/B3</f>
+        <v>122.88</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
this synth, tests are stil todo
</commit_message>
<xml_diff>
--- a/doc/PIN_REVERSE_ENGINEERING.xlsx
+++ b/doc/PIN_REVERSE_ENGINEERING.xlsx
@@ -855,8 +855,8 @@
   </sheetPr>
   <dimension ref="A1:C62"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A58" activeCellId="0" sqref="A58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2273,13 +2273,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D17" activeCellId="0" sqref="D17"/>
+      <selection pane="topLeft" activeCell="D14" activeCellId="0" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.16015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="18.3"/>
@@ -2330,6 +2330,22 @@
       <c r="E3" s="0" t="n">
         <f aca="false">D2/B3</f>
         <v>122.88</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="n">
+        <v>800</v>
+      </c>
+      <c r="B6" s="0" t="n">
+        <f aca="false">1000/A6</f>
+        <v>1.25</v>
+      </c>
+      <c r="C6" s="0" t="n">
+        <v>1024</v>
+      </c>
+      <c r="D6" s="0" t="n">
+        <f aca="false">B6*C6</f>
+        <v>1280</v>
       </c>
     </row>
   </sheetData>

</xml_diff>